<commit_message>
Update correct usernames, improve R detection and formatting of excel template
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -1005,13 +1005,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
@@ -1033,68 +1032,14 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-    </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates from aggregate statistics
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -7,23 +7,24 @@
     <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Applications CPU 2016-11-08" sheetId="1" r:id="rId1"/>
-    <sheet name="User Walltime CPU 2016-10" sheetId="4" r:id="rId2"/>
-    <sheet name="Org HighLevel CPU 2016-10" sheetId="7" r:id="rId3"/>
-    <sheet name="Org Breakdown CPU 2016-10" sheetId="5" r:id="rId4"/>
-    <sheet name="Largest Jobs CPU 2016-10" sheetId="6" r:id="rId5"/>
-    <sheet name="Applications GPU 2016-10" sheetId="3" r:id="rId6"/>
-    <sheet name="User Walltime GPU 2016-10" sheetId="10" r:id="rId7"/>
-    <sheet name="Org HighLevel GPU 2016-10" sheetId="8" r:id="rId8"/>
-    <sheet name="Org Breakdown GPU 2016-10" sheetId="9" r:id="rId9"/>
-    <sheet name="Largest Jobs GPU 2016-10" sheetId="11" r:id="rId10"/>
+    <sheet name="Applications CPU 2016-12-06" sheetId="1" r:id="rId1"/>
+    <sheet name="User Walltime CPU 2016-12-06" sheetId="4" r:id="rId2"/>
+    <sheet name="Org HighLevel CPU 2016-12-06" sheetId="7" r:id="rId3"/>
+    <sheet name="Org Breakdown CPU 2016-12-06" sheetId="5" r:id="rId4"/>
+    <sheet name="Largest Jobs CPU 2016-12-06" sheetId="6" r:id="rId5"/>
+    <sheet name="Applications GPU 2016-12-06" sheetId="3" r:id="rId6"/>
+    <sheet name="User Walltime GPU 2016-12-06" sheetId="10" r:id="rId7"/>
+    <sheet name="Org HighLevel GPU 2016-12-06" sheetId="8" r:id="rId8"/>
+    <sheet name="Org Breakdown GPU 2016-12-06" sheetId="9" r:id="rId9"/>
+    <sheet name="Largest Jobs GPU 2016-12-06" sheetId="11" r:id="rId10"/>
+    <sheet name="Cumulative 2016-12-06 " sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>Rank</t>
   </si>
@@ -65,6 +66,30 @@
   </si>
   <si>
     <t>Wait time</t>
+  </si>
+  <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>A*STAR</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (CPU nodes)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (GPU Nodes)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (Total)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +577,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,6 +602,8 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -630,6 +657,761 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-SG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (CPU nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40330490.090555601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42272318.338611163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61272817.936388962</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80419405.701388955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91797570.830833361</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105082245.94444446</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121867569.14833337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>125709252.57027781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (GPU Nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5033947.3422222203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5180112.3222222207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6788200.1555555509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8659560.7688888814</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11262494.555555552</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13249154.188888881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15551657.535555551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16024845.195555551</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="109089920"/>
+        <c:axId val="109091456"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="109089920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109091456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="109091456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109089920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-SG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A*STAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23684370.820555601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25114494.81444449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34275807.027222268</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41874775.00250005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45743559.290000051</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49915318.677222274</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56129899.423611164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57343464.365000054</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NUS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12013985.7005556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12117030.835000044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17592846.070277825</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24181683.087500043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28231926.511388935</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34904363.028333388</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40616298.492777824</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42044918.803055607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NTU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7310391.2061111098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7746515.088333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12743684.413611112</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18131719.079166673</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20946688.638888892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24377322.916666672</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29517978.718888894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30959033.800555564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2016-12-06 '!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2016-12-06 '!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2355689.7055554884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2474389.9230554923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3448680.5808332525</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4890789.3011109931</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8137890.9461109843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9134395.5111109316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11155050.048610983</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11386680.797222083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="109331200"/>
+        <c:axId val="109332736"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="109331200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109332736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="109332736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109331200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1009,6 +1791,399 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>42457</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>42457</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>42538</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40330490.090555601</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5033947.3422222203</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45364437.4327778</v>
+      </c>
+      <c r="G3" s="13">
+        <v>42538</v>
+      </c>
+      <c r="H3" s="1">
+        <v>23684370.820555601</v>
+      </c>
+      <c r="I3" s="1">
+        <v>12013985.7005556</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7310391.2061111098</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2355689.7055554884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>42551</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42272318.338611163</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5180112.3222222207</v>
+      </c>
+      <c r="D4" s="1">
+        <v>47452430.660833359</v>
+      </c>
+      <c r="G4" s="13">
+        <v>42551</v>
+      </c>
+      <c r="H4" s="1">
+        <v>25114494.81444449</v>
+      </c>
+      <c r="I4" s="1">
+        <v>12117030.835000044</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7746515.088333332</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2474389.9230554923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>42582</v>
+      </c>
+      <c r="B5" s="1">
+        <v>61272817.936388962</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6788200.1555555509</v>
+      </c>
+      <c r="D5" s="1">
+        <v>68061018.091944456</v>
+      </c>
+      <c r="G5" s="13">
+        <v>42582</v>
+      </c>
+      <c r="H5" s="1">
+        <v>34275807.027222268</v>
+      </c>
+      <c r="I5" s="1">
+        <v>17592846.070277825</v>
+      </c>
+      <c r="J5" s="1">
+        <v>12743684.413611112</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3448680.5808332525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>42613</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80419405.701388955</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8659560.7688888814</v>
+      </c>
+      <c r="D6" s="1">
+        <v>89078966.470277756</v>
+      </c>
+      <c r="G6" s="13">
+        <v>42613</v>
+      </c>
+      <c r="H6" s="1">
+        <v>41874775.00250005</v>
+      </c>
+      <c r="I6" s="1">
+        <v>24181683.087500043</v>
+      </c>
+      <c r="J6" s="1">
+        <v>18131719.079166673</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4890789.3011109931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>42643</v>
+      </c>
+      <c r="B7" s="1">
+        <v>91797570.830833361</v>
+      </c>
+      <c r="C7" s="1">
+        <v>11262494.555555552</v>
+      </c>
+      <c r="D7" s="1">
+        <v>103060065.38638885</v>
+      </c>
+      <c r="G7" s="13">
+        <v>42643</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45743559.290000051</v>
+      </c>
+      <c r="I7" s="1">
+        <v>28231926.511388935</v>
+      </c>
+      <c r="J7" s="1">
+        <v>20946688.638888892</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8137890.9461109843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>42674</v>
+      </c>
+      <c r="B8" s="1">
+        <v>105082245.94444446</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13249154.188888881</v>
+      </c>
+      <c r="D8" s="1">
+        <v>118331400.13333325</v>
+      </c>
+      <c r="G8" s="13">
+        <v>42674</v>
+      </c>
+      <c r="H8" s="1">
+        <v>49915318.677222274</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34904363.028333388</v>
+      </c>
+      <c r="J8" s="1">
+        <v>24377322.916666672</v>
+      </c>
+      <c r="K8" s="1">
+        <v>9134395.5111109316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>42704</v>
+      </c>
+      <c r="B9" s="1">
+        <v>121867569.14833337</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15551657.535555551</v>
+      </c>
+      <c r="D9" s="1">
+        <v>137419226.68388885</v>
+      </c>
+      <c r="G9" s="13">
+        <v>42704</v>
+      </c>
+      <c r="H9" s="1">
+        <v>56129899.423611164</v>
+      </c>
+      <c r="I9" s="1">
+        <v>40616298.492777824</v>
+      </c>
+      <c r="J9" s="1">
+        <v>29517978.718888894</v>
+      </c>
+      <c r="K9" s="1">
+        <v>11155050.048610983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>42710</v>
+      </c>
+      <c r="B10" s="1">
+        <v>125709252.57027781</v>
+      </c>
+      <c r="C10" s="1">
+        <v>16024845.195555551</v>
+      </c>
+      <c r="D10" s="1">
+        <v>141734097.76583329</v>
+      </c>
+      <c r="G10" s="13">
+        <v>42710</v>
+      </c>
+      <c r="H10" s="1">
+        <v>57343464.365000054</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42044918.803055607</v>
+      </c>
+      <c r="J10" s="1">
+        <v>30959033.800555564</v>
+      </c>
+      <c r="K10" s="1">
+        <v>11386680.797222083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>

</xml_diff>

<commit_message>
Added wait times grouped by core count
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -4,26 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620" activeTab="11"/>
   </bookViews>
   <sheets>
-    <sheet name="Applications CPU 2016-12-27" sheetId="1" r:id="rId1"/>
-    <sheet name="User Walltime CPU 2016-12-27" sheetId="4" r:id="rId2"/>
-    <sheet name="Org HighLevel CPU 2016-12-27" sheetId="7" r:id="rId3"/>
-    <sheet name="Org Breakdown CPU 2016-12-27" sheetId="5" r:id="rId4"/>
-    <sheet name="Largest Jobs CPU 2016-12-27" sheetId="6" r:id="rId5"/>
-    <sheet name="Applications GPU 2016-12-27" sheetId="3" r:id="rId6"/>
-    <sheet name="User Walltime GPU 2016-12-27" sheetId="10" r:id="rId7"/>
-    <sheet name="Org HighLevel GPU 2016-12-27" sheetId="8" r:id="rId8"/>
-    <sheet name="Org Breakdown GPU 2016-12-27" sheetId="9" r:id="rId9"/>
-    <sheet name="Largest Jobs GPU 2016-12-27" sheetId="11" r:id="rId10"/>
+    <sheet name="By Cores CPU 2016-12" sheetId="15" r:id="rId1"/>
+    <sheet name="Applications CPU 2016-12" sheetId="1" r:id="rId2"/>
+    <sheet name="User Walltime CPU 2016-12" sheetId="4" r:id="rId3"/>
+    <sheet name="Org HighLevel CPU 2016-12-27" sheetId="7" r:id="rId4"/>
+    <sheet name="Org Breakdown CPU 2016-12-27" sheetId="5" r:id="rId5"/>
+    <sheet name="Largest Jobs CPU 2016-12-27" sheetId="6" r:id="rId6"/>
+    <sheet name="By Cores GPU 2016-12" sheetId="16" r:id="rId7"/>
+    <sheet name="Applications GPU 2016-12-27" sheetId="3" r:id="rId8"/>
+    <sheet name="User Walltime GPU 2016-12-27" sheetId="10" r:id="rId9"/>
+    <sheet name="Org HighLevel GPU 2016-12-27" sheetId="8" r:id="rId10"/>
+    <sheet name="Org Breakdown GPU 2016-12-27" sheetId="9" r:id="rId11"/>
+    <sheet name="Largest Jobs GPU 2016-12-27" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
   <si>
     <t>Rank</t>
   </si>
@@ -65,6 +67,30 @@
   </si>
   <si>
     <t>Wait time</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-24</t>
+  </si>
+  <si>
+    <t>25-96</t>
+  </si>
+  <si>
+    <t>97-240</t>
+  </si>
+  <si>
+    <t>241-960</t>
+  </si>
+  <si>
+    <t>&gt;960</t>
+  </si>
+  <si>
+    <t>Median Wait (hrs)</t>
+  </si>
+  <si>
+    <t>Mean Wait (hrs)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,6 +603,13 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,34 +952,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -957,9 +1020,97 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1011,6 +1162,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1044,50 +1233,6 @@
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1141,6 +1286,50 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1193,7 +1382,77 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -1235,7 +1494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1275,92 +1534,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for GPU-based statistics
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -4,28 +4,29 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620"/>
+    <workbookView xWindow="2700" yWindow="-105" windowWidth="19155" windowHeight="7620" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
-    <sheet name="By Cores CPU 2017-03-28" sheetId="15" r:id="rId1"/>
-    <sheet name="Applications CPU 2017-03-28" sheetId="1" r:id="rId2"/>
-    <sheet name="User Walltime CPU 2017-03-28" sheetId="4" r:id="rId3"/>
-    <sheet name="Org HighLevel CPU 2017-03-28" sheetId="7" r:id="rId4"/>
-    <sheet name="Org Breakdown CPU 2017-03-28" sheetId="5" r:id="rId5"/>
-    <sheet name="Largest Jobs CPU 2017-03-28" sheetId="6" r:id="rId6"/>
-    <sheet name="By Cores GPU 2017-03-28" sheetId="16" r:id="rId7"/>
-    <sheet name="Applications GPU 2017-03-28" sheetId="3" r:id="rId8"/>
-    <sheet name="User Walltime GPU 2017-03-28" sheetId="10" r:id="rId9"/>
-    <sheet name="Org HighLevel GPU 2017-03-28" sheetId="8" r:id="rId10"/>
-    <sheet name="Org Breakdown GPU 2017-03-28" sheetId="9" r:id="rId11"/>
-    <sheet name="Largest Jobs GPU 2017-03-28" sheetId="11" r:id="rId12"/>
+    <sheet name="Active Users 2017-04-25" sheetId="17" r:id="rId1"/>
+    <sheet name="By Cores CPU 2017-04-25" sheetId="15" r:id="rId2"/>
+    <sheet name="Applications CPU 2017-04-25" sheetId="1" r:id="rId3"/>
+    <sheet name="User Walltime CPU 2017-04-25" sheetId="4" r:id="rId4"/>
+    <sheet name="Org HighLevel CPU 2017-04-25" sheetId="7" r:id="rId5"/>
+    <sheet name="Org Breakdown CPU 2017-04-25" sheetId="5" r:id="rId6"/>
+    <sheet name="Largest Jobs CPU 2017-04-25" sheetId="6" r:id="rId7"/>
+    <sheet name="By GPU 2017-04-25" sheetId="16" r:id="rId8"/>
+    <sheet name="Applications GPU 2017-04-25" sheetId="3" r:id="rId9"/>
+    <sheet name="User Walltime GPU 2017-04-25" sheetId="10" r:id="rId10"/>
+    <sheet name="Org HighLevel GPU 2017-04-25" sheetId="8" r:id="rId11"/>
+    <sheet name="Org Breakdown GPU 2017-04-25" sheetId="9" r:id="rId12"/>
+    <sheet name="Largest Jobs GPU 2017-04-25" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Rank</t>
   </si>
@@ -93,16 +94,52 @@
     <t>24</t>
   </si>
   <si>
-    <t>48-96</t>
-  </si>
-  <si>
-    <t>120-240</t>
-  </si>
-  <si>
-    <t>264-960</t>
-  </si>
-  <si>
     <t>2-23</t>
+  </si>
+  <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>SUTD</t>
+  </si>
+  <si>
+    <t>CREATE</t>
+  </si>
+  <si>
+    <t>A*STAR</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>GPUs</t>
+  </si>
+  <si>
+    <t>GPUs*walltime(hrs)</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>11-40</t>
+  </si>
+  <si>
+    <t>&gt;40</t>
+  </si>
+  <si>
+    <t>GPU Hours</t>
+  </si>
+  <si>
+    <t>Active Users</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -430,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -545,6 +582,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -590,7 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -622,6 +688,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -964,70 +1035,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="18"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1037,41 +1102,42 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1101,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1112,6 +1178,9 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
@@ -1124,6 +1193,367 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1177,231 +1607,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1414,15 +1622,15 @@
     <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>19</v>
@@ -1431,30 +1639,34 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>18</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,9 +1674,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1485,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1498,47 +1710,8 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated excel template and added top application for each user
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -4,29 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="-105" windowWidth="19155" windowHeight="7620" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Active Users 2017-04-25" sheetId="17" r:id="rId1"/>
-    <sheet name="By Cores CPU 2017-04-25" sheetId="15" r:id="rId2"/>
-    <sheet name="Applications CPU 2017-04-25" sheetId="1" r:id="rId3"/>
-    <sheet name="User Walltime CPU 2017-04-25" sheetId="4" r:id="rId4"/>
-    <sheet name="Org HighLevel CPU 2017-04-25" sheetId="7" r:id="rId5"/>
-    <sheet name="Org Breakdown CPU 2017-04-25" sheetId="5" r:id="rId6"/>
-    <sheet name="Largest Jobs CPU 2017-04-25" sheetId="6" r:id="rId7"/>
-    <sheet name="By GPU 2017-04-25" sheetId="16" r:id="rId8"/>
-    <sheet name="Applications GPU 2017-04-25" sheetId="3" r:id="rId9"/>
-    <sheet name="User Walltime GPU 2017-04-25" sheetId="10" r:id="rId10"/>
-    <sheet name="Org HighLevel GPU 2017-04-25" sheetId="8" r:id="rId11"/>
-    <sheet name="Org Breakdown GPU 2017-04-25" sheetId="9" r:id="rId12"/>
-    <sheet name="Largest Jobs GPU 2017-04-25" sheetId="11" r:id="rId13"/>
+    <sheet name="Storage By Org 2017-06-20" sheetId="19" r:id="rId1"/>
+    <sheet name="Active Users 2017-06-20" sheetId="18" r:id="rId2"/>
+    <sheet name="By Cores CPU 2017-06-20" sheetId="15" r:id="rId3"/>
+    <sheet name="Applications CPU 2017-06-20" sheetId="1" r:id="rId4"/>
+    <sheet name="User Walltime CPU 2017-06-20" sheetId="4" r:id="rId5"/>
+    <sheet name="Org HighLevel CPU 2017-06-20" sheetId="7" r:id="rId6"/>
+    <sheet name="Org Breakdown CPU 2017-06-20" sheetId="5" r:id="rId7"/>
+    <sheet name="Largest Jobs CPU 2017-06-20" sheetId="6" r:id="rId8"/>
+    <sheet name="By Cores GPU 2017-06-20" sheetId="16" r:id="rId9"/>
+    <sheet name="Applications GPU 2017-06-20" sheetId="3" r:id="rId10"/>
+    <sheet name="User Walltime GPU 2017-06-20" sheetId="10" r:id="rId11"/>
+    <sheet name="Org HighLevel GPU 2017-06-20" sheetId="8" r:id="rId12"/>
+    <sheet name="Org Breakdown GPU 2017-06-20" sheetId="9" r:id="rId13"/>
+    <sheet name="Largest Jobs GPU 2017-06-20" sheetId="11" r:id="rId14"/>
+    <sheet name="Cumulative 2017-06" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>Rank</t>
   </si>
@@ -70,6 +72,18 @@
     <t>Wait time</t>
   </si>
   <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>A*STAR</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -97,10 +111,7 @@
     <t>2-23</t>
   </si>
   <si>
-    <t>NUS</t>
-  </si>
-  <si>
-    <t>NTU</t>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>SUTD</t>
@@ -109,18 +120,39 @@
     <t>CREATE</t>
   </si>
   <si>
-    <t>A*STAR</t>
-  </si>
-  <si>
-    <t>Other</t>
+    <t>Active Users</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>seq (TB)</t>
+  </si>
+  <si>
+    <t>home (TB)</t>
+  </si>
+  <si>
+    <t>home1 (TB)</t>
+  </si>
+  <si>
+    <t>scratch (TB)</t>
+  </si>
+  <si>
+    <t>secure (TB)</t>
+  </si>
+  <si>
+    <t>Total (TB)</t>
+  </si>
+  <si>
+    <t>Top Application</t>
+  </si>
+  <si>
+    <t>GPUs*walltime(hrs)</t>
   </si>
   <si>
     <t>GPUs</t>
   </si>
   <si>
-    <t>GPUs*walltime(hrs)</t>
-  </si>
-  <si>
     <t>2-4</t>
   </si>
   <si>
@@ -136,18 +168,25 @@
     <t>GPU Hours</t>
   </si>
   <si>
-    <t>Active Users</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (Total)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (GPU Nodes)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (CPU nodes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -467,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -596,6 +635,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -603,9 +651,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -656,7 +710,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -690,9 +744,18 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -746,6 +809,761 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-SG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (CPU nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40330490.090555601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42272318.338611163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61272817.936388962</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80419405.701388955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91797570.830833361</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105082245.94444446</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121867569.14833337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>125709252.57027781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (GPU Nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5033947.3422222203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5180112.3222222207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6788200.1555555509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8659560.7688888814</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11262494.555555552</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13249154.188888881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15551657.535555551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16024845.195555551</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="129661952"/>
+        <c:axId val="129684224"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="129661952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129684224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="129684224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129661952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-SG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A*STAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23684370.820555601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25114494.81444449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34275807.027222268</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41874775.00250005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45743559.290000051</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49915318.677222274</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56129899.423611164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57343464.365000054</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NUS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12013985.7005556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12117030.835000044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17592846.070277825</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24181683.087500043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28231926.511388935</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34904363.028333388</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40616298.492777824</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42044918.803055607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NTU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7310391.2061111098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7746515.088333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12743684.413611112</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18131719.079166673</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20946688.638888892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24377322.916666672</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29517978.718888894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30959033.800555564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2017-06'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2017-06'!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2355689.7055554884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2474389.9230554923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3448680.5808332525</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4890789.3011109931</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8137890.9461109843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9134395.5111109316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11155050.048610983</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11386680.797222083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="129772160"/>
+        <c:axId val="129786240"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="129772160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129786240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="129786240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129772160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1035,64 +1853,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="F1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="21" t="e">
+        <f t="shared" ref="H2:H7" si="0">G2/G$8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="16"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="17"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="18"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="18"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="23">
+        <f t="shared" ref="B8:G8" si="1">SUM(B2:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1102,7 +2019,49 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1114,9 +2073,10 @@
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1130,61 +2090,17 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1214,7 +2130,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1225,10 +2141,6 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
@@ -1241,223 +2153,6 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J13" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -1468,7 +2163,6 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1480,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1491,9 +2185,6 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F10" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
@@ -1505,55 +2196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1578,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -1593,7 +2236,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>12</v>
@@ -1607,9 +2250,766 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>42457</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="26">
+        <v>42457</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>42538</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40330490.090555601</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5033947.3422222203</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45364437.4327778</v>
+      </c>
+      <c r="G3" s="26">
+        <v>42538</v>
+      </c>
+      <c r="H3" s="1">
+        <v>23684370.820555601</v>
+      </c>
+      <c r="I3" s="1">
+        <v>12013985.7005556</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7310391.2061111098</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2355689.7055554884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>42551</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42272318.338611163</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5180112.3222222207</v>
+      </c>
+      <c r="D4" s="1">
+        <v>47452430.660833359</v>
+      </c>
+      <c r="G4" s="26">
+        <v>42551</v>
+      </c>
+      <c r="H4" s="1">
+        <v>25114494.81444449</v>
+      </c>
+      <c r="I4" s="1">
+        <v>12117030.835000044</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7746515.088333332</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2474389.9230554923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>42582</v>
+      </c>
+      <c r="B5" s="1">
+        <v>61272817.936388962</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6788200.1555555509</v>
+      </c>
+      <c r="D5" s="1">
+        <v>68061018.091944456</v>
+      </c>
+      <c r="G5" s="26">
+        <v>42582</v>
+      </c>
+      <c r="H5" s="1">
+        <v>34275807.027222268</v>
+      </c>
+      <c r="I5" s="1">
+        <v>17592846.070277825</v>
+      </c>
+      <c r="J5" s="1">
+        <v>12743684.413611112</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3448680.5808332525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>42613</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80419405.701388955</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8659560.7688888814</v>
+      </c>
+      <c r="D6" s="1">
+        <v>89078966.470277756</v>
+      </c>
+      <c r="G6" s="26">
+        <v>42613</v>
+      </c>
+      <c r="H6" s="1">
+        <v>41874775.00250005</v>
+      </c>
+      <c r="I6" s="1">
+        <v>24181683.087500043</v>
+      </c>
+      <c r="J6" s="1">
+        <v>18131719.079166673</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4890789.3011109931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>42643</v>
+      </c>
+      <c r="B7" s="1">
+        <v>91797570.830833361</v>
+      </c>
+      <c r="C7" s="1">
+        <v>11262494.555555552</v>
+      </c>
+      <c r="D7" s="1">
+        <v>103060065.38638885</v>
+      </c>
+      <c r="G7" s="26">
+        <v>42643</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45743559.290000051</v>
+      </c>
+      <c r="I7" s="1">
+        <v>28231926.511388935</v>
+      </c>
+      <c r="J7" s="1">
+        <v>20946688.638888892</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8137890.9461109843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>42674</v>
+      </c>
+      <c r="B8" s="1">
+        <v>105082245.94444446</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13249154.188888881</v>
+      </c>
+      <c r="D8" s="1">
+        <v>118331400.13333325</v>
+      </c>
+      <c r="G8" s="26">
+        <v>42674</v>
+      </c>
+      <c r="H8" s="1">
+        <v>49915318.677222274</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34904363.028333388</v>
+      </c>
+      <c r="J8" s="1">
+        <v>24377322.916666672</v>
+      </c>
+      <c r="K8" s="1">
+        <v>9134395.5111109316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>42704</v>
+      </c>
+      <c r="B9" s="1">
+        <v>121867569.14833337</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15551657.535555551</v>
+      </c>
+      <c r="D9" s="1">
+        <v>137419226.68388885</v>
+      </c>
+      <c r="G9" s="26">
+        <v>42704</v>
+      </c>
+      <c r="H9" s="1">
+        <v>56129899.423611164</v>
+      </c>
+      <c r="I9" s="1">
+        <v>40616298.492777824</v>
+      </c>
+      <c r="J9" s="1">
+        <v>29517978.718888894</v>
+      </c>
+      <c r="K9" s="1">
+        <v>11155050.048610983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>42710</v>
+      </c>
+      <c r="B10" s="1">
+        <v>125709252.57027781</v>
+      </c>
+      <c r="C10" s="1">
+        <v>16024845.195555551</v>
+      </c>
+      <c r="D10" s="1">
+        <v>141734097.76583329</v>
+      </c>
+      <c r="G10" s="26">
+        <v>42710</v>
+      </c>
+      <c r="H10" s="1">
+        <v>57343464.365000054</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42044918.803055607</v>
+      </c>
+      <c r="J10" s="1">
+        <v>30959033.800555564</v>
+      </c>
+      <c r="K10" s="1">
+        <v>11386680.797222083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1622,96 +3022,47 @@
     <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Excel template with enhanced project information
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
   <si>
     <t>Rank</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>Industry &amp; Other</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>Project Description</t>
   </si>
 </sst>
 </file>
@@ -1165,11 +1171,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147727104"/>
-        <c:axId val="147728640"/>
+        <c:axId val="94285824"/>
+        <c:axId val="94287360"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="147727104"/>
+        <c:axId val="94285824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,14 +1185,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147728640"/>
+        <c:crossAx val="94287360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="147728640"/>
+        <c:axId val="94287360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,7 +1203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147727104"/>
+        <c:crossAx val="94285824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1936,11 +1942,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147772544"/>
-        <c:axId val="147774080"/>
+        <c:axId val="112067712"/>
+        <c:axId val="112101248"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="147772544"/>
+        <c:axId val="112067712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,14 +1956,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147774080"/>
+        <c:crossAx val="112101248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="147774080"/>
+        <c:axId val="112101248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,14 +1974,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147772544"/>
+        <c:crossAx val="112067712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2346,7 +2351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2357,9 +2362,11 @@
     <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="7" max="7" width="139.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2375,50 +2382,56 @@
       <c r="E1" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update instructions and excel template
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -34,13 +34,17 @@
     <sheet name="Org HighLevel GPU 2018-09-18" sheetId="8" r:id="rId20"/>
     <sheet name="Org Breakdown GPU 2018-09-18" sheetId="9" r:id="rId21"/>
     <sheet name="Largest Jobs GPU 2018-09-18" sheetId="11" r:id="rId22"/>
+    <sheet name="Cumulative 2018-09" sheetId="35" r:id="rId23"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId24"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
   <si>
     <t>Rank</t>
   </si>
@@ -304,6 +308,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (CPU nodes)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (GPU Nodes)</t>
+  </si>
+  <si>
+    <t>Cumulative Core Hours (Total)</t>
+  </si>
+  <si>
+    <t>Industry &amp; Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -966,6 +988,2750 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16387806175390868"/>
+          <c:y val="4.6044656805630302E-2"/>
+          <c:w val="0.52474812741430577"/>
+          <c:h val="0.72330329479134559"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (CPU nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41515601.188611098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43498600.438611098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62390934.264722198</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81475607.481944397</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92635599.422777802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>106419986.16944399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>122841353.38249999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>138637852.47166699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>157230950.66666701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>174764740.83388901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>192916055.90444401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>211720916.744167</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230919864.221111</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>249005189.67611101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>266936676.198333</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>283593104.57305598</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>300152017.509444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>315965584.54722202</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>333997098.63277799</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>348846197.60861099</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>364624503.01027799</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>381574647.875278</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>398824226.78027803</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>416307445.14555597</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>434557785.78250003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>450423475.024167</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>469270269.675556</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>488706241.62138933</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>503869057.607521</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D24B-49B4-AB45-FDF60374071D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Core Hours (GPU Nodes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4660208.0666666701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4805520.4666666696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6358490.3399999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8241452.8133333297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10736001.206666701</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12901314.813333301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15094269.893333299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16949466.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19036381.719999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20859964.006666701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22772028.053333301</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24724853.393333301</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26808345.413333301</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28703917.5666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30758431.2266667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32609443.153333299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34178264.460000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>35718879.32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37371036.293333299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38729788.68</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40145114.227222197</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41917944.731944397</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43499917.205277801</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45446290.738611102</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>47136106.211944401</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>48215932.985277802</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>49511659.351944402</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>50577905.091944404</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>52039647.698611103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D24B-49B4-AB45-FDF60374071D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="113592576"/>
+        <c:axId val="113606656"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="113592576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ yyyy" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113606656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="113606656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113592576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73845234298983653"/>
+          <c:y val="0.37489550297032809"/>
+          <c:w val="0.24908659782013229"/>
+          <c:h val="0.25020899405934388"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15963526403859712"/>
+          <c:y val="4.926241928152654E-2"/>
+          <c:w val="0.59398924648981988"/>
+          <c:h val="0.70396675637423956"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A*STAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$H$2:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24562569.515277799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26033013.509166699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35247387.720833302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42825018.751111098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46666274.1297222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51249853.161666699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57154144.860277802</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61703314.560555503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67549377.876944393</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71947097.201944396</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76357104.516388893</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81375155.1875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86161436.9491667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>91275614.107777804</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97287676.206944406</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>103347500.76222201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>109591660.463889</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>114790148.4025</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>121782633.35111099</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>127386474.815833</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>134477576.67833301</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>142794104.42583299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>150222427.68472201</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>157273143.93583301</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>163186233.11277801</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>169853770.068333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>179359531.591389</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>187883964.14583343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>194280827.72224301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B42A-4019-B390-FEC487DD91F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NUS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$I$2:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11228948.621111101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11331993.7555556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16744875.6163889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23370843.7341667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27266987.3172222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34068271.007222198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39740736.366388902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46925795.598611102</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55768722.152777798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62004571.033611096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67740808.998611093</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74111826.151944295</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80462450.331666604</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87141287.7444444</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>94531390.963055506</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100799107.66722199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>107399896.805555</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>113964339.644722</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>119955238.375833</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>125851241.096111</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>131696426.081389</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>138146044.161111</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>145921210.45444399</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>153957364.223611</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>163148270.90916699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>169781806.67222199</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>176869249.916944</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>185464750.9841662</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>191644649.90083301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B42A-4019-B390-FEC487DD91F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NTU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$J$2:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7310084.4550000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7746208.3372222204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12579036.4344444</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17946711.326388899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20640594.2938889</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24174804.7658333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29212454.633055601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34400492.978888899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39697985.619166702</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47850468.612222202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56683705.698611103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64764006.681111097</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>74105917.465833396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>81629134.457777798</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87135446.443611205</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>91598582.373611197</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>94740092.928055599</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99203029.090833396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>103673356.33499999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>107563684.542778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>111098146.941945</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>113915163.38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>116192065.97972199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>118968182.76444501</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>121669606.1925</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>123969022.83611099</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>125884336.710833</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>128260702.37666632</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>130808713.873889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B42A-4019-B390-FEC487DD91F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CREATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$K$2:$K$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1537410.0674999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1574657.4275</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2415334.6847222201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3662462.9030555598</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4880822.5555555597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5552614.5863888897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7232936.4583333302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7695489.9961111099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7789645.5427777804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7905387.9894444402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8194858.1861111103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8472312.8783333302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8699092.5716666691</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8741999.3183333296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9206129.6316666696</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9752514.4116666708</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10793443.284166699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11056978.467222201</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12288510.884722199</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12709121.3647222</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12822636.038055601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13019589.838055599</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13232770.5391667</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13427362.826388899</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13988384.3458333</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14299679.685000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14393674.0033333</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14524236.5233333</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14731818.5133333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B42A-4019-B390-FEC487DD91F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative 2018-09'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Industry &amp; Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>42457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative 2018-09'!$L$2:$L$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1536796.5963900001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1618247.87583</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1762790.14833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1912023.5805599999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3916922.3330600001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4275757.4616700001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4595350.9577799998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4862225.8375000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5461601.1950000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5917180.0033299997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6711606.5580599997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7722469.2386100003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8299312.31611</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8921071.6144399997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9534464.1797199994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10704842.511670001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11805188.487779999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12669968.261940001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13668395.97944</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14065464.46917</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14674831.497780001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15617690.80222</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16755669.327500001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18127682.133889999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19701397.434166599</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20735128.747779999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22275136.805</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23150492.68333447</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24442695.29583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B42A-4019-B390-FEC487DD91F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="114104960"/>
+        <c:axId val="114106752"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="114104960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ yyyy" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114106752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="114106752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114104960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Queue First Job 2018-09"/>
+      <sheetName val="Core Summary 2018-09"/>
+      <sheetName val="Project Usage 2018-09"/>
+      <sheetName val="Project Stakeholder 2018-09"/>
+      <sheetName val="Project Status 2018-09"/>
+      <sheetName val="Personal Status 2018-09"/>
+      <sheetName val="Storage Summary 2018-09"/>
+      <sheetName val="Storage by Fileset 2018-09"/>
+      <sheetName val="Storage By Org 2018-09"/>
+      <sheetName val="Active Users 2018-09"/>
+      <sheetName val="By Cores CPU 2018-09"/>
+      <sheetName val="Applications CPU 2018-09"/>
+      <sheetName val="User Walltime CPU 2018-09"/>
+      <sheetName val="Org HighLevel CPU 2018-09"/>
+      <sheetName val="Org Breakdown CPU 2018-09"/>
+      <sheetName val="Largest Jobs CPU 2018-09"/>
+      <sheetName val="By Cores GPU 2018-09"/>
+      <sheetName val="Applications GPU 2018-09"/>
+      <sheetName val="User Walltime GPU 2018-09"/>
+      <sheetName val="Org HighLevel GPU 2018-09"/>
+      <sheetName val="Org Breakdown GPU 2018-09"/>
+      <sheetName val="Largest Jobs GPU 2018-09"/>
+      <sheetName val="Cumulative 2018-09"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Cumulative Core Hours (CPU nodes)</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Cumulative Core Hours (GPU Nodes)</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>A*STAR</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>NUS</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>NTU</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>CREATE</v>
+          </cell>
+          <cell r="L1" t="str">
+            <v>Industry &amp; Other</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>42457</v>
+          </cell>
+          <cell r="B2">
+            <v>0</v>
+          </cell>
+          <cell r="C2">
+            <v>0</v>
+          </cell>
+          <cell r="G2">
+            <v>42457</v>
+          </cell>
+          <cell r="H2">
+            <v>0</v>
+          </cell>
+          <cell r="I2">
+            <v>0</v>
+          </cell>
+          <cell r="J2">
+            <v>0</v>
+          </cell>
+          <cell r="K2">
+            <v>0</v>
+          </cell>
+          <cell r="L2">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>42538</v>
+          </cell>
+          <cell r="B3">
+            <v>41515601.188611098</v>
+          </cell>
+          <cell r="C3">
+            <v>4660208.0666666701</v>
+          </cell>
+          <cell r="G3">
+            <v>42538</v>
+          </cell>
+          <cell r="H3">
+            <v>24562569.515277799</v>
+          </cell>
+          <cell r="I3">
+            <v>11228948.621111101</v>
+          </cell>
+          <cell r="J3">
+            <v>7310084.4550000001</v>
+          </cell>
+          <cell r="K3">
+            <v>1537410.0674999999</v>
+          </cell>
+          <cell r="L3">
+            <v>1536796.5963900001</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>42551</v>
+          </cell>
+          <cell r="B4">
+            <v>43498600.438611098</v>
+          </cell>
+          <cell r="C4">
+            <v>4805520.4666666696</v>
+          </cell>
+          <cell r="G4">
+            <v>42551</v>
+          </cell>
+          <cell r="H4">
+            <v>26033013.509166699</v>
+          </cell>
+          <cell r="I4">
+            <v>11331993.7555556</v>
+          </cell>
+          <cell r="J4">
+            <v>7746208.3372222204</v>
+          </cell>
+          <cell r="K4">
+            <v>1574657.4275</v>
+          </cell>
+          <cell r="L4">
+            <v>1618247.87583</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>42582</v>
+          </cell>
+          <cell r="B5">
+            <v>62390934.264722198</v>
+          </cell>
+          <cell r="C5">
+            <v>6358490.3399999999</v>
+          </cell>
+          <cell r="G5">
+            <v>42582</v>
+          </cell>
+          <cell r="H5">
+            <v>35247387.720833302</v>
+          </cell>
+          <cell r="I5">
+            <v>16744875.6163889</v>
+          </cell>
+          <cell r="J5">
+            <v>12579036.4344444</v>
+          </cell>
+          <cell r="K5">
+            <v>2415334.6847222201</v>
+          </cell>
+          <cell r="L5">
+            <v>1762790.14833</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>42613</v>
+          </cell>
+          <cell r="B6">
+            <v>81475607.481944397</v>
+          </cell>
+          <cell r="C6">
+            <v>8241452.8133333297</v>
+          </cell>
+          <cell r="G6">
+            <v>42613</v>
+          </cell>
+          <cell r="H6">
+            <v>42825018.751111098</v>
+          </cell>
+          <cell r="I6">
+            <v>23370843.7341667</v>
+          </cell>
+          <cell r="J6">
+            <v>17946711.326388899</v>
+          </cell>
+          <cell r="K6">
+            <v>3662462.9030555598</v>
+          </cell>
+          <cell r="L6">
+            <v>1912023.5805599999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>42643</v>
+          </cell>
+          <cell r="B7">
+            <v>92635599.422777802</v>
+          </cell>
+          <cell r="C7">
+            <v>10736001.206666701</v>
+          </cell>
+          <cell r="G7">
+            <v>42643</v>
+          </cell>
+          <cell r="H7">
+            <v>46666274.1297222</v>
+          </cell>
+          <cell r="I7">
+            <v>27266987.3172222</v>
+          </cell>
+          <cell r="J7">
+            <v>20640594.2938889</v>
+          </cell>
+          <cell r="K7">
+            <v>4880822.5555555597</v>
+          </cell>
+          <cell r="L7">
+            <v>3916922.3330600001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>42674</v>
+          </cell>
+          <cell r="B8">
+            <v>106419986.16944399</v>
+          </cell>
+          <cell r="C8">
+            <v>12901314.813333301</v>
+          </cell>
+          <cell r="G8">
+            <v>42674</v>
+          </cell>
+          <cell r="H8">
+            <v>51249853.161666699</v>
+          </cell>
+          <cell r="I8">
+            <v>34068271.007222198</v>
+          </cell>
+          <cell r="J8">
+            <v>24174804.7658333</v>
+          </cell>
+          <cell r="K8">
+            <v>5552614.5863888897</v>
+          </cell>
+          <cell r="L8">
+            <v>4275757.4616700001</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>42704</v>
+          </cell>
+          <cell r="B9">
+            <v>122841353.38249999</v>
+          </cell>
+          <cell r="C9">
+            <v>15094269.893333299</v>
+          </cell>
+          <cell r="G9">
+            <v>42704</v>
+          </cell>
+          <cell r="H9">
+            <v>57154144.860277802</v>
+          </cell>
+          <cell r="I9">
+            <v>39740736.366388902</v>
+          </cell>
+          <cell r="J9">
+            <v>29212454.633055601</v>
+          </cell>
+          <cell r="K9">
+            <v>7232936.4583333302</v>
+          </cell>
+          <cell r="L9">
+            <v>4595350.9577799998</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>42735</v>
+          </cell>
+          <cell r="B10">
+            <v>138637852.47166699</v>
+          </cell>
+          <cell r="C10">
+            <v>16949466.5</v>
+          </cell>
+          <cell r="G10">
+            <v>42735</v>
+          </cell>
+          <cell r="H10">
+            <v>61703314.560555503</v>
+          </cell>
+          <cell r="I10">
+            <v>46925795.598611102</v>
+          </cell>
+          <cell r="J10">
+            <v>34400492.978888899</v>
+          </cell>
+          <cell r="K10">
+            <v>7695489.9961111099</v>
+          </cell>
+          <cell r="L10">
+            <v>4862225.8375000004</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>42766</v>
+          </cell>
+          <cell r="B11">
+            <v>157230950.66666701</v>
+          </cell>
+          <cell r="C11">
+            <v>19036381.719999999</v>
+          </cell>
+          <cell r="G11">
+            <v>42766</v>
+          </cell>
+          <cell r="H11">
+            <v>67549377.876944393</v>
+          </cell>
+          <cell r="I11">
+            <v>55768722.152777798</v>
+          </cell>
+          <cell r="J11">
+            <v>39697985.619166702</v>
+          </cell>
+          <cell r="K11">
+            <v>7789645.5427777804</v>
+          </cell>
+          <cell r="L11">
+            <v>5461601.1950000003</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>42794</v>
+          </cell>
+          <cell r="B12">
+            <v>174764740.83388901</v>
+          </cell>
+          <cell r="C12">
+            <v>20859964.006666701</v>
+          </cell>
+          <cell r="G12">
+            <v>42794</v>
+          </cell>
+          <cell r="H12">
+            <v>71947097.201944396</v>
+          </cell>
+          <cell r="I12">
+            <v>62004571.033611096</v>
+          </cell>
+          <cell r="J12">
+            <v>47850468.612222202</v>
+          </cell>
+          <cell r="K12">
+            <v>7905387.9894444402</v>
+          </cell>
+          <cell r="L12">
+            <v>5917180.0033299997</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>42825</v>
+          </cell>
+          <cell r="B13">
+            <v>192916055.90444401</v>
+          </cell>
+          <cell r="C13">
+            <v>22772028.053333301</v>
+          </cell>
+          <cell r="G13">
+            <v>42825</v>
+          </cell>
+          <cell r="H13">
+            <v>76357104.516388893</v>
+          </cell>
+          <cell r="I13">
+            <v>67740808.998611093</v>
+          </cell>
+          <cell r="J13">
+            <v>56683705.698611103</v>
+          </cell>
+          <cell r="K13">
+            <v>8194858.1861111103</v>
+          </cell>
+          <cell r="L13">
+            <v>6711606.5580599997</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>42855</v>
+          </cell>
+          <cell r="B14">
+            <v>211720916.744167</v>
+          </cell>
+          <cell r="C14">
+            <v>24724853.393333301</v>
+          </cell>
+          <cell r="G14">
+            <v>42855</v>
+          </cell>
+          <cell r="H14">
+            <v>81375155.1875</v>
+          </cell>
+          <cell r="I14">
+            <v>74111826.151944295</v>
+          </cell>
+          <cell r="J14">
+            <v>64764006.681111097</v>
+          </cell>
+          <cell r="K14">
+            <v>8472312.8783333302</v>
+          </cell>
+          <cell r="L14">
+            <v>7722469.2386100003</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>42886</v>
+          </cell>
+          <cell r="B15">
+            <v>230919864.221111</v>
+          </cell>
+          <cell r="C15">
+            <v>26808345.413333301</v>
+          </cell>
+          <cell r="G15">
+            <v>42886</v>
+          </cell>
+          <cell r="H15">
+            <v>86161436.9491667</v>
+          </cell>
+          <cell r="I15">
+            <v>80462450.331666604</v>
+          </cell>
+          <cell r="J15">
+            <v>74105917.465833396</v>
+          </cell>
+          <cell r="K15">
+            <v>8699092.5716666691</v>
+          </cell>
+          <cell r="L15">
+            <v>8299312.31611</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>42916</v>
+          </cell>
+          <cell r="B16">
+            <v>249005189.67611101</v>
+          </cell>
+          <cell r="C16">
+            <v>28703917.5666667</v>
+          </cell>
+          <cell r="G16">
+            <v>42916</v>
+          </cell>
+          <cell r="H16">
+            <v>91275614.107777804</v>
+          </cell>
+          <cell r="I16">
+            <v>87141287.7444444</v>
+          </cell>
+          <cell r="J16">
+            <v>81629134.457777798</v>
+          </cell>
+          <cell r="K16">
+            <v>8741999.3183333296</v>
+          </cell>
+          <cell r="L16">
+            <v>8921071.6144399997</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>42947</v>
+          </cell>
+          <cell r="B17">
+            <v>266936676.198333</v>
+          </cell>
+          <cell r="C17">
+            <v>30758431.2266667</v>
+          </cell>
+          <cell r="G17">
+            <v>42947</v>
+          </cell>
+          <cell r="H17">
+            <v>97287676.206944406</v>
+          </cell>
+          <cell r="I17">
+            <v>94531390.963055506</v>
+          </cell>
+          <cell r="J17">
+            <v>87135446.443611205</v>
+          </cell>
+          <cell r="K17">
+            <v>9206129.6316666696</v>
+          </cell>
+          <cell r="L17">
+            <v>9534464.1797199994</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>42978</v>
+          </cell>
+          <cell r="B18">
+            <v>283593104.57305598</v>
+          </cell>
+          <cell r="C18">
+            <v>32609443.153333299</v>
+          </cell>
+          <cell r="G18">
+            <v>42978</v>
+          </cell>
+          <cell r="H18">
+            <v>103347500.76222201</v>
+          </cell>
+          <cell r="I18">
+            <v>100799107.66722199</v>
+          </cell>
+          <cell r="J18">
+            <v>91598582.373611197</v>
+          </cell>
+          <cell r="K18">
+            <v>9752514.4116666708</v>
+          </cell>
+          <cell r="L18">
+            <v>10704842.511670001</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>43008</v>
+          </cell>
+          <cell r="B19">
+            <v>300152017.509444</v>
+          </cell>
+          <cell r="C19">
+            <v>34178264.460000001</v>
+          </cell>
+          <cell r="G19">
+            <v>43008</v>
+          </cell>
+          <cell r="H19">
+            <v>109591660.463889</v>
+          </cell>
+          <cell r="I19">
+            <v>107399896.805555</v>
+          </cell>
+          <cell r="J19">
+            <v>94740092.928055599</v>
+          </cell>
+          <cell r="K19">
+            <v>10793443.284166699</v>
+          </cell>
+          <cell r="L19">
+            <v>11805188.487779999</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>43039</v>
+          </cell>
+          <cell r="B20">
+            <v>315965584.54722202</v>
+          </cell>
+          <cell r="C20">
+            <v>35718879.32</v>
+          </cell>
+          <cell r="G20">
+            <v>43039</v>
+          </cell>
+          <cell r="H20">
+            <v>114790148.4025</v>
+          </cell>
+          <cell r="I20">
+            <v>113964339.644722</v>
+          </cell>
+          <cell r="J20">
+            <v>99203029.090833396</v>
+          </cell>
+          <cell r="K20">
+            <v>11056978.467222201</v>
+          </cell>
+          <cell r="L20">
+            <v>12669968.261940001</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>43069</v>
+          </cell>
+          <cell r="B21">
+            <v>333997098.63277799</v>
+          </cell>
+          <cell r="C21">
+            <v>37371036.293333299</v>
+          </cell>
+          <cell r="G21">
+            <v>43069</v>
+          </cell>
+          <cell r="H21">
+            <v>121782633.35111099</v>
+          </cell>
+          <cell r="I21">
+            <v>119955238.375833</v>
+          </cell>
+          <cell r="J21">
+            <v>103673356.33499999</v>
+          </cell>
+          <cell r="K21">
+            <v>12288510.884722199</v>
+          </cell>
+          <cell r="L21">
+            <v>13668395.97944</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>43100</v>
+          </cell>
+          <cell r="B22">
+            <v>348846197.60861099</v>
+          </cell>
+          <cell r="C22">
+            <v>38729788.68</v>
+          </cell>
+          <cell r="G22">
+            <v>43100</v>
+          </cell>
+          <cell r="H22">
+            <v>127386474.815833</v>
+          </cell>
+          <cell r="I22">
+            <v>125851241.096111</v>
+          </cell>
+          <cell r="J22">
+            <v>107563684.542778</v>
+          </cell>
+          <cell r="K22">
+            <v>12709121.3647222</v>
+          </cell>
+          <cell r="L22">
+            <v>14065464.46917</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>43131</v>
+          </cell>
+          <cell r="B23">
+            <v>364624503.01027799</v>
+          </cell>
+          <cell r="C23">
+            <v>40145114.227222197</v>
+          </cell>
+          <cell r="G23">
+            <v>43131</v>
+          </cell>
+          <cell r="H23">
+            <v>134477576.67833301</v>
+          </cell>
+          <cell r="I23">
+            <v>131696426.081389</v>
+          </cell>
+          <cell r="J23">
+            <v>111098146.941945</v>
+          </cell>
+          <cell r="K23">
+            <v>12822636.038055601</v>
+          </cell>
+          <cell r="L23">
+            <v>14674831.497780001</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>43159</v>
+          </cell>
+          <cell r="B24">
+            <v>381574647.875278</v>
+          </cell>
+          <cell r="C24">
+            <v>41917944.731944397</v>
+          </cell>
+          <cell r="G24">
+            <v>43159</v>
+          </cell>
+          <cell r="H24">
+            <v>142794104.42583299</v>
+          </cell>
+          <cell r="I24">
+            <v>138146044.161111</v>
+          </cell>
+          <cell r="J24">
+            <v>113915163.38</v>
+          </cell>
+          <cell r="K24">
+            <v>13019589.838055599</v>
+          </cell>
+          <cell r="L24">
+            <v>15617690.80222</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>43190</v>
+          </cell>
+          <cell r="B25">
+            <v>398824226.78027803</v>
+          </cell>
+          <cell r="C25">
+            <v>43499917.205277801</v>
+          </cell>
+          <cell r="G25">
+            <v>43190</v>
+          </cell>
+          <cell r="H25">
+            <v>150222427.68472201</v>
+          </cell>
+          <cell r="I25">
+            <v>145921210.45444399</v>
+          </cell>
+          <cell r="J25">
+            <v>116192065.97972199</v>
+          </cell>
+          <cell r="K25">
+            <v>13232770.5391667</v>
+          </cell>
+          <cell r="L25">
+            <v>16755669.327500001</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>43220</v>
+          </cell>
+          <cell r="B26">
+            <v>416307445.14555597</v>
+          </cell>
+          <cell r="C26">
+            <v>45446290.738611102</v>
+          </cell>
+          <cell r="G26">
+            <v>43220</v>
+          </cell>
+          <cell r="H26">
+            <v>157273143.93583301</v>
+          </cell>
+          <cell r="I26">
+            <v>153957364.223611</v>
+          </cell>
+          <cell r="J26">
+            <v>118968182.76444501</v>
+          </cell>
+          <cell r="K26">
+            <v>13427362.826388899</v>
+          </cell>
+          <cell r="L26">
+            <v>18127682.133889999</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>43251</v>
+          </cell>
+          <cell r="B27">
+            <v>434557785.78250003</v>
+          </cell>
+          <cell r="C27">
+            <v>47136106.211944401</v>
+          </cell>
+          <cell r="G27">
+            <v>43251</v>
+          </cell>
+          <cell r="H27">
+            <v>163186233.11277801</v>
+          </cell>
+          <cell r="I27">
+            <v>163148270.90916699</v>
+          </cell>
+          <cell r="J27">
+            <v>121669606.1925</v>
+          </cell>
+          <cell r="K27">
+            <v>13988384.3458333</v>
+          </cell>
+          <cell r="L27">
+            <v>19701397.434166599</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>43281</v>
+          </cell>
+          <cell r="B28">
+            <v>450423475.024167</v>
+          </cell>
+          <cell r="C28">
+            <v>48215932.985277802</v>
+          </cell>
+          <cell r="G28">
+            <v>43281</v>
+          </cell>
+          <cell r="H28">
+            <v>169853770.068333</v>
+          </cell>
+          <cell r="I28">
+            <v>169781806.67222199</v>
+          </cell>
+          <cell r="J28">
+            <v>123969022.83611099</v>
+          </cell>
+          <cell r="K28">
+            <v>14299679.685000001</v>
+          </cell>
+          <cell r="L28">
+            <v>20735128.747779999</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>43312</v>
+          </cell>
+          <cell r="B29">
+            <v>469270269.675556</v>
+          </cell>
+          <cell r="C29">
+            <v>49511659.351944402</v>
+          </cell>
+          <cell r="G29">
+            <v>43312</v>
+          </cell>
+          <cell r="H29">
+            <v>179359531.591389</v>
+          </cell>
+          <cell r="I29">
+            <v>176869249.916944</v>
+          </cell>
+          <cell r="J29">
+            <v>125884336.710833</v>
+          </cell>
+          <cell r="K29">
+            <v>14393674.0033333</v>
+          </cell>
+          <cell r="L29">
+            <v>22275136.805</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>43343</v>
+          </cell>
+          <cell r="B30">
+            <v>488706241.62138933</v>
+          </cell>
+          <cell r="C30">
+            <v>50577905.091944404</v>
+          </cell>
+          <cell r="G30">
+            <v>43343</v>
+          </cell>
+          <cell r="H30">
+            <v>187883964.14583343</v>
+          </cell>
+          <cell r="I30">
+            <v>185464750.9841662</v>
+          </cell>
+          <cell r="J30">
+            <v>128260702.37666632</v>
+          </cell>
+          <cell r="K30">
+            <v>14524236.5233333</v>
+          </cell>
+          <cell r="L30">
+            <v>23150492.68333447</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>43373</v>
+          </cell>
+          <cell r="B31">
+            <v>503869057.607521</v>
+          </cell>
+          <cell r="C31">
+            <v>52039647.698611103</v>
+          </cell>
+          <cell r="G31">
+            <v>43373</v>
+          </cell>
+          <cell r="H31">
+            <v>194280827.72224301</v>
+          </cell>
+          <cell r="I31">
+            <v>191644649.90083301</v>
+          </cell>
+          <cell r="J31">
+            <v>130808713.873889</v>
+          </cell>
+          <cell r="K31">
+            <v>14731818.5133333</v>
+          </cell>
+          <cell r="L31">
+            <v>24442695.29583</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2579,6 +5345,1165 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="15" style="31" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="39" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="32" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="32" customWidth="1"/>
+    <col min="10" max="12" width="15" style="32" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>42457</v>
+      </c>
+      <c r="B2" s="32">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="G2" s="21">
+        <v>42457</v>
+      </c>
+      <c r="H2" s="32">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32">
+        <v>0</v>
+      </c>
+      <c r="J2" s="32">
+        <v>0</v>
+      </c>
+      <c r="K2" s="32">
+        <v>0</v>
+      </c>
+      <c r="L2" s="32">
+        <v>0</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>42538</v>
+      </c>
+      <c r="B3" s="32">
+        <v>41515601.188611098</v>
+      </c>
+      <c r="C3" s="32">
+        <v>4660208.0666666701</v>
+      </c>
+      <c r="D3" s="32">
+        <v>46175809.255277798</v>
+      </c>
+      <c r="G3" s="21">
+        <v>42538</v>
+      </c>
+      <c r="H3" s="32">
+        <v>24562569.515277799</v>
+      </c>
+      <c r="I3" s="32">
+        <v>11228948.621111101</v>
+      </c>
+      <c r="J3" s="32">
+        <v>7310084.4550000001</v>
+      </c>
+      <c r="K3" s="32">
+        <v>1537410.0674999999</v>
+      </c>
+      <c r="L3" s="32">
+        <v>1536796.5963900001</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>42551</v>
+      </c>
+      <c r="B4" s="32">
+        <v>43498600.438611098</v>
+      </c>
+      <c r="C4" s="32">
+        <v>4805520.4666666696</v>
+      </c>
+      <c r="D4" s="32">
+        <v>48304120.905277804</v>
+      </c>
+      <c r="G4" s="21">
+        <v>42551</v>
+      </c>
+      <c r="H4" s="32">
+        <v>26033013.509166699</v>
+      </c>
+      <c r="I4" s="32">
+        <v>11331993.7555556</v>
+      </c>
+      <c r="J4" s="32">
+        <v>7746208.3372222204</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1574657.4275</v>
+      </c>
+      <c r="L4" s="32">
+        <v>1618247.87583</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>42582</v>
+      </c>
+      <c r="B5" s="32">
+        <v>62390934.264722198</v>
+      </c>
+      <c r="C5" s="32">
+        <v>6358490.3399999999</v>
+      </c>
+      <c r="D5" s="32">
+        <v>68749424.604722202</v>
+      </c>
+      <c r="G5" s="21">
+        <v>42582</v>
+      </c>
+      <c r="H5" s="32">
+        <v>35247387.720833302</v>
+      </c>
+      <c r="I5" s="32">
+        <v>16744875.6163889</v>
+      </c>
+      <c r="J5" s="32">
+        <v>12579036.4344444</v>
+      </c>
+      <c r="K5" s="32">
+        <v>2415334.6847222201</v>
+      </c>
+      <c r="L5" s="32">
+        <v>1762790.14833</v>
+      </c>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>42613</v>
+      </c>
+      <c r="B6" s="32">
+        <v>81475607.481944397</v>
+      </c>
+      <c r="C6" s="32">
+        <v>8241452.8133333297</v>
+      </c>
+      <c r="D6" s="32">
+        <v>89717060.295277804</v>
+      </c>
+      <c r="G6" s="21">
+        <v>42613</v>
+      </c>
+      <c r="H6" s="32">
+        <v>42825018.751111098</v>
+      </c>
+      <c r="I6" s="32">
+        <v>23370843.7341667</v>
+      </c>
+      <c r="J6" s="32">
+        <v>17946711.326388899</v>
+      </c>
+      <c r="K6" s="32">
+        <v>3662462.9030555598</v>
+      </c>
+      <c r="L6" s="32">
+        <v>1912023.5805599999</v>
+      </c>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>42643</v>
+      </c>
+      <c r="B7" s="32">
+        <v>92635599.422777802</v>
+      </c>
+      <c r="C7" s="32">
+        <v>10736001.206666701</v>
+      </c>
+      <c r="D7" s="32">
+        <v>103371600.629444</v>
+      </c>
+      <c r="G7" s="21">
+        <v>42643</v>
+      </c>
+      <c r="H7" s="32">
+        <v>46666274.1297222</v>
+      </c>
+      <c r="I7" s="32">
+        <v>27266987.3172222</v>
+      </c>
+      <c r="J7" s="32">
+        <v>20640594.2938889</v>
+      </c>
+      <c r="K7" s="32">
+        <v>4880822.5555555597</v>
+      </c>
+      <c r="L7" s="32">
+        <v>3916922.3330600001</v>
+      </c>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>42674</v>
+      </c>
+      <c r="B8" s="32">
+        <v>106419986.16944399</v>
+      </c>
+      <c r="C8" s="32">
+        <v>12901314.813333301</v>
+      </c>
+      <c r="D8" s="32">
+        <v>119321300.982778</v>
+      </c>
+      <c r="G8" s="21">
+        <v>42674</v>
+      </c>
+      <c r="H8" s="32">
+        <v>51249853.161666699</v>
+      </c>
+      <c r="I8" s="32">
+        <v>34068271.007222198</v>
+      </c>
+      <c r="J8" s="32">
+        <v>24174804.7658333</v>
+      </c>
+      <c r="K8" s="32">
+        <v>5552614.5863888897</v>
+      </c>
+      <c r="L8" s="32">
+        <v>4275757.4616700001</v>
+      </c>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>42704</v>
+      </c>
+      <c r="B9" s="32">
+        <v>122841353.38249999</v>
+      </c>
+      <c r="C9" s="32">
+        <v>15094269.893333299</v>
+      </c>
+      <c r="D9" s="32">
+        <v>137935623.27583301</v>
+      </c>
+      <c r="G9" s="21">
+        <v>42704</v>
+      </c>
+      <c r="H9" s="32">
+        <v>57154144.860277802</v>
+      </c>
+      <c r="I9" s="32">
+        <v>39740736.366388902</v>
+      </c>
+      <c r="J9" s="32">
+        <v>29212454.633055601</v>
+      </c>
+      <c r="K9" s="32">
+        <v>7232936.4583333302</v>
+      </c>
+      <c r="L9" s="32">
+        <v>4595350.9577799998</v>
+      </c>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>42735</v>
+      </c>
+      <c r="B10" s="32">
+        <v>138637852.47166699</v>
+      </c>
+      <c r="C10" s="32">
+        <v>16949466.5</v>
+      </c>
+      <c r="D10" s="32">
+        <v>155587318.97166699</v>
+      </c>
+      <c r="G10" s="21">
+        <v>42735</v>
+      </c>
+      <c r="H10" s="32">
+        <v>61703314.560555503</v>
+      </c>
+      <c r="I10" s="32">
+        <v>46925795.598611102</v>
+      </c>
+      <c r="J10" s="32">
+        <v>34400492.978888899</v>
+      </c>
+      <c r="K10" s="32">
+        <v>7695489.9961111099</v>
+      </c>
+      <c r="L10" s="32">
+        <v>4862225.8375000004</v>
+      </c>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>42766</v>
+      </c>
+      <c r="B11" s="32">
+        <v>157230950.66666701</v>
+      </c>
+      <c r="C11" s="32">
+        <v>19036381.719999999</v>
+      </c>
+      <c r="D11" s="32">
+        <v>176267332.38666701</v>
+      </c>
+      <c r="G11" s="21">
+        <v>42766</v>
+      </c>
+      <c r="H11" s="32">
+        <v>67549377.876944393</v>
+      </c>
+      <c r="I11" s="32">
+        <v>55768722.152777798</v>
+      </c>
+      <c r="J11" s="32">
+        <v>39697985.619166702</v>
+      </c>
+      <c r="K11" s="32">
+        <v>7789645.5427777804</v>
+      </c>
+      <c r="L11" s="32">
+        <v>5461601.1950000003</v>
+      </c>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>42794</v>
+      </c>
+      <c r="B12" s="32">
+        <v>174764740.83388901</v>
+      </c>
+      <c r="C12" s="32">
+        <v>20859964.006666701</v>
+      </c>
+      <c r="D12" s="32">
+        <v>195624704.840556</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="G12" s="21">
+        <v>42794</v>
+      </c>
+      <c r="H12" s="32">
+        <v>71947097.201944396</v>
+      </c>
+      <c r="I12" s="32">
+        <v>62004571.033611096</v>
+      </c>
+      <c r="J12" s="32">
+        <v>47850468.612222202</v>
+      </c>
+      <c r="K12" s="32">
+        <v>7905387.9894444402</v>
+      </c>
+      <c r="L12" s="32">
+        <v>5917180.0033299997</v>
+      </c>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>42825</v>
+      </c>
+      <c r="B13" s="32">
+        <v>192916055.90444401</v>
+      </c>
+      <c r="C13" s="32">
+        <v>22772028.053333301</v>
+      </c>
+      <c r="D13" s="32">
+        <v>215688083.95777801</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="G13" s="21">
+        <v>42825</v>
+      </c>
+      <c r="H13" s="32">
+        <v>76357104.516388893</v>
+      </c>
+      <c r="I13" s="32">
+        <v>67740808.998611093</v>
+      </c>
+      <c r="J13" s="32">
+        <v>56683705.698611103</v>
+      </c>
+      <c r="K13" s="32">
+        <v>8194858.1861111103</v>
+      </c>
+      <c r="L13" s="32">
+        <v>6711606.5580599997</v>
+      </c>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>42855</v>
+      </c>
+      <c r="B14" s="32">
+        <v>211720916.744167</v>
+      </c>
+      <c r="C14" s="32">
+        <v>24724853.393333301</v>
+      </c>
+      <c r="D14" s="32">
+        <v>236445770.13749999</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="G14" s="21">
+        <v>42855</v>
+      </c>
+      <c r="H14" s="32">
+        <v>81375155.1875</v>
+      </c>
+      <c r="I14" s="32">
+        <v>74111826.151944295</v>
+      </c>
+      <c r="J14" s="32">
+        <v>64764006.681111097</v>
+      </c>
+      <c r="K14" s="32">
+        <v>8472312.8783333302</v>
+      </c>
+      <c r="L14" s="32">
+        <v>7722469.2386100003</v>
+      </c>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>42886</v>
+      </c>
+      <c r="B15" s="32">
+        <v>230919864.221111</v>
+      </c>
+      <c r="C15" s="32">
+        <v>26808345.413333301</v>
+      </c>
+      <c r="D15" s="32">
+        <v>257728209.634444</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="G15" s="21">
+        <v>42886</v>
+      </c>
+      <c r="H15" s="32">
+        <v>86161436.9491667</v>
+      </c>
+      <c r="I15" s="32">
+        <v>80462450.331666604</v>
+      </c>
+      <c r="J15" s="32">
+        <v>74105917.465833396</v>
+      </c>
+      <c r="K15" s="32">
+        <v>8699092.5716666691</v>
+      </c>
+      <c r="L15" s="32">
+        <v>8299312.31611</v>
+      </c>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>42916</v>
+      </c>
+      <c r="B16" s="32">
+        <v>249005189.67611101</v>
+      </c>
+      <c r="C16" s="32">
+        <v>28703917.5666667</v>
+      </c>
+      <c r="D16" s="32">
+        <v>277709107.242778</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="G16" s="21">
+        <v>42916</v>
+      </c>
+      <c r="H16" s="32">
+        <v>91275614.107777804</v>
+      </c>
+      <c r="I16" s="32">
+        <v>87141287.7444444</v>
+      </c>
+      <c r="J16" s="32">
+        <v>81629134.457777798</v>
+      </c>
+      <c r="K16" s="32">
+        <v>8741999.3183333296</v>
+      </c>
+      <c r="L16" s="32">
+        <v>8921071.6144399997</v>
+      </c>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>42947</v>
+      </c>
+      <c r="B17" s="32">
+        <v>266936676.198333</v>
+      </c>
+      <c r="C17" s="32">
+        <v>30758431.2266667</v>
+      </c>
+      <c r="D17" s="32">
+        <v>297695107.42500001</v>
+      </c>
+      <c r="G17" s="21">
+        <v>42947</v>
+      </c>
+      <c r="H17" s="32">
+        <v>97287676.206944406</v>
+      </c>
+      <c r="I17" s="32">
+        <v>94531390.963055506</v>
+      </c>
+      <c r="J17" s="32">
+        <v>87135446.443611205</v>
+      </c>
+      <c r="K17" s="32">
+        <v>9206129.6316666696</v>
+      </c>
+      <c r="L17" s="32">
+        <v>9534464.1797199994</v>
+      </c>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>42978</v>
+      </c>
+      <c r="B18" s="32">
+        <v>283593104.57305598</v>
+      </c>
+      <c r="C18" s="32">
+        <v>32609443.153333299</v>
+      </c>
+      <c r="D18" s="32">
+        <v>316202547.72638899</v>
+      </c>
+      <c r="G18" s="21">
+        <v>42978</v>
+      </c>
+      <c r="H18" s="32">
+        <v>103347500.76222201</v>
+      </c>
+      <c r="I18" s="32">
+        <v>100799107.66722199</v>
+      </c>
+      <c r="J18" s="32">
+        <v>91598582.373611197</v>
+      </c>
+      <c r="K18" s="32">
+        <v>9752514.4116666708</v>
+      </c>
+      <c r="L18" s="32">
+        <v>10704842.511670001</v>
+      </c>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>43008</v>
+      </c>
+      <c r="B19" s="32">
+        <v>300152017.509444</v>
+      </c>
+      <c r="C19" s="32">
+        <v>34178264.460000001</v>
+      </c>
+      <c r="D19" s="32">
+        <v>334330281.96944398</v>
+      </c>
+      <c r="G19" s="21">
+        <v>43008</v>
+      </c>
+      <c r="H19" s="32">
+        <v>109591660.463889</v>
+      </c>
+      <c r="I19" s="32">
+        <v>107399896.805555</v>
+      </c>
+      <c r="J19" s="32">
+        <v>94740092.928055599</v>
+      </c>
+      <c r="K19" s="32">
+        <v>10793443.284166699</v>
+      </c>
+      <c r="L19" s="32">
+        <v>11805188.487779999</v>
+      </c>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>43039</v>
+      </c>
+      <c r="B20" s="32">
+        <v>315965584.54722202</v>
+      </c>
+      <c r="C20" s="32">
+        <v>35718879.32</v>
+      </c>
+      <c r="D20" s="32">
+        <v>351684463.86722201</v>
+      </c>
+      <c r="G20" s="21">
+        <v>43039</v>
+      </c>
+      <c r="H20" s="32">
+        <v>114790148.4025</v>
+      </c>
+      <c r="I20" s="32">
+        <v>113964339.644722</v>
+      </c>
+      <c r="J20" s="32">
+        <v>99203029.090833396</v>
+      </c>
+      <c r="K20" s="32">
+        <v>11056978.467222201</v>
+      </c>
+      <c r="L20" s="32">
+        <v>12669968.261940001</v>
+      </c>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>43069</v>
+      </c>
+      <c r="B21" s="32">
+        <v>333997098.63277799</v>
+      </c>
+      <c r="C21" s="32">
+        <v>37371036.293333299</v>
+      </c>
+      <c r="D21" s="32">
+        <v>371368134.92611098</v>
+      </c>
+      <c r="G21" s="21">
+        <v>43069</v>
+      </c>
+      <c r="H21" s="32">
+        <v>121782633.35111099</v>
+      </c>
+      <c r="I21" s="32">
+        <v>119955238.375833</v>
+      </c>
+      <c r="J21" s="32">
+        <v>103673356.33499999</v>
+      </c>
+      <c r="K21" s="32">
+        <v>12288510.884722199</v>
+      </c>
+      <c r="L21" s="32">
+        <v>13668395.97944</v>
+      </c>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>43100</v>
+      </c>
+      <c r="B22" s="32">
+        <v>348846197.60861099</v>
+      </c>
+      <c r="C22" s="32">
+        <v>38729788.68</v>
+      </c>
+      <c r="D22" s="32">
+        <v>387575986.28861099</v>
+      </c>
+      <c r="G22" s="21">
+        <v>43100</v>
+      </c>
+      <c r="H22" s="32">
+        <v>127386474.815833</v>
+      </c>
+      <c r="I22" s="32">
+        <v>125851241.096111</v>
+      </c>
+      <c r="J22" s="32">
+        <v>107563684.542778</v>
+      </c>
+      <c r="K22" s="32">
+        <v>12709121.3647222</v>
+      </c>
+      <c r="L22" s="32">
+        <v>14065464.46917</v>
+      </c>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>43131</v>
+      </c>
+      <c r="B23" s="32">
+        <v>364624503.01027799</v>
+      </c>
+      <c r="C23" s="32">
+        <v>40145114.227222197</v>
+      </c>
+      <c r="D23" s="32">
+        <v>404769617.23750001</v>
+      </c>
+      <c r="G23" s="21">
+        <v>43131</v>
+      </c>
+      <c r="H23" s="32">
+        <v>134477576.67833301</v>
+      </c>
+      <c r="I23" s="32">
+        <v>131696426.081389</v>
+      </c>
+      <c r="J23" s="32">
+        <v>111098146.941945</v>
+      </c>
+      <c r="K23" s="32">
+        <v>12822636.038055601</v>
+      </c>
+      <c r="L23" s="32">
+        <v>14674831.497780001</v>
+      </c>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <v>43159</v>
+      </c>
+      <c r="B24" s="32">
+        <v>381574647.875278</v>
+      </c>
+      <c r="C24" s="32">
+        <v>41917944.731944397</v>
+      </c>
+      <c r="D24" s="32">
+        <v>423492592.60722202</v>
+      </c>
+      <c r="G24" s="21">
+        <v>43159</v>
+      </c>
+      <c r="H24" s="32">
+        <v>142794104.42583299</v>
+      </c>
+      <c r="I24" s="32">
+        <v>138146044.161111</v>
+      </c>
+      <c r="J24" s="32">
+        <v>113915163.38</v>
+      </c>
+      <c r="K24" s="32">
+        <v>13019589.838055599</v>
+      </c>
+      <c r="L24" s="32">
+        <v>15617690.80222</v>
+      </c>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>43190</v>
+      </c>
+      <c r="B25" s="32">
+        <v>398824226.78027803</v>
+      </c>
+      <c r="C25" s="32">
+        <v>43499917.205277801</v>
+      </c>
+      <c r="D25" s="32">
+        <v>442324143.98555601</v>
+      </c>
+      <c r="G25" s="21">
+        <v>43190</v>
+      </c>
+      <c r="H25" s="32">
+        <v>150222427.68472201</v>
+      </c>
+      <c r="I25" s="32">
+        <v>145921210.45444399</v>
+      </c>
+      <c r="J25" s="32">
+        <v>116192065.97972199</v>
+      </c>
+      <c r="K25" s="32">
+        <v>13232770.5391667</v>
+      </c>
+      <c r="L25" s="32">
+        <v>16755669.327500001</v>
+      </c>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>43220</v>
+      </c>
+      <c r="B26" s="32">
+        <v>416307445.14555597</v>
+      </c>
+      <c r="C26" s="32">
+        <v>45446290.738611102</v>
+      </c>
+      <c r="D26" s="32">
+        <v>461753735.88416702</v>
+      </c>
+      <c r="G26" s="21">
+        <v>43220</v>
+      </c>
+      <c r="H26" s="32">
+        <v>157273143.93583301</v>
+      </c>
+      <c r="I26" s="32">
+        <v>153957364.223611</v>
+      </c>
+      <c r="J26" s="32">
+        <v>118968182.76444501</v>
+      </c>
+      <c r="K26" s="32">
+        <v>13427362.826388899</v>
+      </c>
+      <c r="L26" s="32">
+        <v>18127682.133889999</v>
+      </c>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>43251</v>
+      </c>
+      <c r="B27" s="32">
+        <v>434557785.78250003</v>
+      </c>
+      <c r="C27" s="32">
+        <v>47136106.211944401</v>
+      </c>
+      <c r="D27" s="32">
+        <v>481693891.99444503</v>
+      </c>
+      <c r="G27" s="21">
+        <v>43251</v>
+      </c>
+      <c r="H27" s="32">
+        <v>163186233.11277801</v>
+      </c>
+      <c r="I27" s="32">
+        <v>163148270.90916699</v>
+      </c>
+      <c r="J27" s="32">
+        <v>121669606.1925</v>
+      </c>
+      <c r="K27" s="32">
+        <v>13988384.3458333</v>
+      </c>
+      <c r="L27" s="32">
+        <v>19701397.434166599</v>
+      </c>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>43281</v>
+      </c>
+      <c r="B28" s="32">
+        <v>450423475.024167</v>
+      </c>
+      <c r="C28" s="32">
+        <v>48215932.985277802</v>
+      </c>
+      <c r="D28" s="32">
+        <v>498639408.009444</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G28" s="21">
+        <v>43281</v>
+      </c>
+      <c r="H28" s="32">
+        <v>169853770.068333</v>
+      </c>
+      <c r="I28" s="32">
+        <v>169781806.67222199</v>
+      </c>
+      <c r="J28" s="32">
+        <v>123969022.83611099</v>
+      </c>
+      <c r="K28" s="32">
+        <v>14299679.685000001</v>
+      </c>
+      <c r="L28" s="32">
+        <v>20735128.747779999</v>
+      </c>
+      <c r="N28" s="32"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <v>43312</v>
+      </c>
+      <c r="B29" s="32">
+        <v>469270269.675556</v>
+      </c>
+      <c r="C29" s="32">
+        <v>49511659.351944402</v>
+      </c>
+      <c r="D29" s="32">
+        <v>518781929.02749997</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="21">
+        <v>43312</v>
+      </c>
+      <c r="H29" s="32">
+        <v>179359531.591389</v>
+      </c>
+      <c r="I29" s="32">
+        <v>176869249.916944</v>
+      </c>
+      <c r="J29" s="32">
+        <v>125884336.710833</v>
+      </c>
+      <c r="K29" s="32">
+        <v>14393674.0033333</v>
+      </c>
+      <c r="L29" s="32">
+        <v>22275136.805</v>
+      </c>
+      <c r="N29" s="32"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>43343</v>
+      </c>
+      <c r="B30" s="32">
+        <v>488706241.62138933</v>
+      </c>
+      <c r="C30" s="32">
+        <v>50577905.091944404</v>
+      </c>
+      <c r="D30" s="32">
+        <v>539284146.71333373</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="21">
+        <v>43343</v>
+      </c>
+      <c r="H30" s="32">
+        <v>187883964.14583343</v>
+      </c>
+      <c r="I30" s="32">
+        <v>185464750.9841662</v>
+      </c>
+      <c r="J30" s="32">
+        <v>128260702.37666632</v>
+      </c>
+      <c r="K30" s="32">
+        <v>14524236.5233333</v>
+      </c>
+      <c r="L30" s="32">
+        <v>23150492.68333447</v>
+      </c>
+      <c r="N30" s="32"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>43373</v>
+      </c>
+      <c r="B31" s="32">
+        <v>503869057.607521</v>
+      </c>
+      <c r="C31" s="32">
+        <v>52039647.698611103</v>
+      </c>
+      <c r="D31" s="32">
+        <v>555908705.30613196</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="21">
+        <v>43373</v>
+      </c>
+      <c r="H31" s="32">
+        <v>194280827.72224301</v>
+      </c>
+      <c r="I31" s="32">
+        <v>191644649.90083301</v>
+      </c>
+      <c r="J31" s="32">
+        <v>130808713.873889</v>
+      </c>
+      <c r="K31" s="32">
+        <v>14731818.5133333</v>
+      </c>
+      <c r="L31" s="32">
+        <v>24442695.29583</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="32"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="32"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="32"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="32"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="32"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="32"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="32"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
@@ -14584,7 +18509,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="16" t="e">
-        <f>G2/G$11</f>
+        <f t="shared" ref="H2:H10" si="0">G2/G$11</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14599,7 +18524,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="16" t="e">
-        <f>G3/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14614,7 +18539,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="18"/>
       <c r="H4" s="16" t="e">
-        <f>G4/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14629,7 +18554,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="16" t="e">
-        <f>G5/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14644,7 +18569,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="18"/>
       <c r="H6" s="16" t="e">
-        <f>G6/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14659,7 +18584,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="18"/>
       <c r="H7" s="16" t="e">
-        <f>G7/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14674,7 +18599,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="18"/>
       <c r="H8" s="16" t="e">
-        <f>G8/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14689,7 +18614,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="18"/>
       <c r="H9" s="16" t="e">
-        <f>G9/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14704,7 +18629,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="16" t="e">
-        <f>G10/G$11</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14713,27 +18638,27 @@
         <v>19</v>
       </c>
       <c r="B11" s="18">
-        <f t="shared" ref="B11:G11" si="0">SUM(B2:B10)</f>
+        <f t="shared" ref="B11:G11" si="1">SUM(B2:B10)</f>
         <v>0</v>
       </c>
       <c r="C11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="16"/>

</xml_diff>

<commit_message>
Auto-completion of a worksheet in Excel spreadsheet
</commit_message>
<xml_diff>
--- a/application_usage-template.xlsx
+++ b/application_usage-template.xlsx
@@ -12,35 +12,35 @@
     <workbookView xWindow="240" yWindow="240" windowWidth="19155" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Queue First Job 2019-02" sheetId="26" r:id="rId1"/>
-    <sheet name="Core Summary 2019-02" sheetId="30" r:id="rId2"/>
-    <sheet name="Project Usage 2019-02" sheetId="23" r:id="rId3"/>
-    <sheet name="Project Stakeholder 2019-02" sheetId="31" r:id="rId4"/>
-    <sheet name="Project Status 2019-02" sheetId="25" r:id="rId5"/>
-    <sheet name="Personal Status 2019-02" sheetId="24" r:id="rId6"/>
-    <sheet name="Storage Summary 2019-02" sheetId="34" r:id="rId7"/>
-    <sheet name="Storage by Fileset 2019-02" sheetId="33" r:id="rId8"/>
-    <sheet name="Storage By Org 2019-02" sheetId="19" r:id="rId9"/>
-    <sheet name="Active Users 2019-02" sheetId="18" r:id="rId10"/>
-    <sheet name="By Cores CPU 2019-02" sheetId="15" r:id="rId11"/>
-    <sheet name="Applications CPU 2019-02" sheetId="1" r:id="rId12"/>
-    <sheet name="User Walltime CPU 2019-02" sheetId="4" r:id="rId13"/>
-    <sheet name="Project CPU 2019-02" sheetId="40" r:id="rId14"/>
-    <sheet name="Org HighLevel CPU 2019-02" sheetId="7" r:id="rId15"/>
-    <sheet name="Org Breakdown CPU 2019-02" sheetId="5" r:id="rId16"/>
-    <sheet name="Largest Jobs CPU 2019-02" sheetId="6" r:id="rId17"/>
-    <sheet name="By Cores GPU 2019-02" sheetId="16" r:id="rId18"/>
-    <sheet name="Applications GPU 2019-02" sheetId="3" r:id="rId19"/>
-    <sheet name="User Walltime GPU 2019-02" sheetId="10" r:id="rId20"/>
-    <sheet name="Project Summary GPU 2019-02" sheetId="41" r:id="rId21"/>
-    <sheet name="Org HighLevel GPU 2019-02" sheetId="8" r:id="rId22"/>
-    <sheet name="Org Breakdown GPU 2019-02" sheetId="9" r:id="rId23"/>
-    <sheet name="Largest Jobs GPU 2019-02" sheetId="11" r:id="rId24"/>
-    <sheet name="Cumulative 2019-02" sheetId="42" r:id="rId25"/>
-    <sheet name="ApplicationsDGX 2019-02" sheetId="36" r:id="rId26"/>
-    <sheet name="User DGX 2019-02" sheetId="37" r:id="rId27"/>
-    <sheet name="Projects DGX 2019-02" sheetId="38" r:id="rId28"/>
-    <sheet name="Org Breakdown DGX 2019-02" sheetId="39" r:id="rId29"/>
+    <sheet name="Queue First Job" sheetId="26" r:id="rId1"/>
+    <sheet name="Core Summary" sheetId="30" r:id="rId2"/>
+    <sheet name="Project Usage" sheetId="23" r:id="rId3"/>
+    <sheet name="Project Stakeholder" sheetId="31" r:id="rId4"/>
+    <sheet name="Project Status" sheetId="25" r:id="rId5"/>
+    <sheet name="Personal Status" sheetId="24" r:id="rId6"/>
+    <sheet name="Storage Summary" sheetId="34" r:id="rId7"/>
+    <sheet name="Storage by Fileset" sheetId="33" r:id="rId8"/>
+    <sheet name="Storage By Org" sheetId="19" r:id="rId9"/>
+    <sheet name="Active Users" sheetId="18" r:id="rId10"/>
+    <sheet name="By Cores CPU" sheetId="15" r:id="rId11"/>
+    <sheet name="Applications CPU" sheetId="1" r:id="rId12"/>
+    <sheet name="User Walltime CPU" sheetId="4" r:id="rId13"/>
+    <sheet name="Project CPU" sheetId="40" r:id="rId14"/>
+    <sheet name="Org HighLevel CPU" sheetId="7" r:id="rId15"/>
+    <sheet name="Org Breakdown CPU" sheetId="5" r:id="rId16"/>
+    <sheet name="Largest Jobs CPU" sheetId="6" r:id="rId17"/>
+    <sheet name="By Cores GPU" sheetId="16" r:id="rId18"/>
+    <sheet name="Applications GPU" sheetId="3" r:id="rId19"/>
+    <sheet name="User Walltime GPU" sheetId="10" r:id="rId20"/>
+    <sheet name="Project GPU" sheetId="41" r:id="rId21"/>
+    <sheet name="Org HighLevel GPU" sheetId="8" r:id="rId22"/>
+    <sheet name="Org Breakdown GPU" sheetId="9" r:id="rId23"/>
+    <sheet name="Largest Jobs GPU" sheetId="11" r:id="rId24"/>
+    <sheet name="Cumulative" sheetId="42" r:id="rId25"/>
+    <sheet name="ApplicationsDGX" sheetId="36" r:id="rId26"/>
+    <sheet name="User DGX" sheetId="37" r:id="rId27"/>
+    <sheet name="Projects DGX" sheetId="38" r:id="rId28"/>
+    <sheet name="Org Breakdown DGX" sheetId="39" r:id="rId29"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1116,7 +1116,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$B$1</c:f>
+              <c:f>Cumulative!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1127,7 +1127,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$A$2:$A$35</c:f>
+              <c:f>Cumulative!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1238,7 +1238,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$B$2:$B$35</c:f>
+              <c:f>Cumulative!$B$2:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1358,7 +1358,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$C$1</c:f>
+              <c:f>Cumulative!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1369,7 +1369,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$A$2:$A$35</c:f>
+              <c:f>Cumulative!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1480,7 +1480,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$C$2:$C$35</c:f>
+              <c:f>Cumulative!$C$2:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1600,7 +1600,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$F$1</c:f>
+              <c:f>Cumulative!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1616,7 +1616,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$A$2:$A$35</c:f>
+              <c:f>Cumulative!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1727,7 +1727,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$F$2:$F$35</c:f>
+              <c:f>Cumulative!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1948,7 +1948,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$J$1</c:f>
+              <c:f>Cumulative!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1959,7 +1959,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$I$2:$I$35</c:f>
+              <c:f>Cumulative!$I$2:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2070,7 +2070,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$J$2:$J$35</c:f>
+              <c:f>Cumulative!$J$2:$J$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2190,7 +2190,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$K$1</c:f>
+              <c:f>Cumulative!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2201,7 +2201,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$I$2:$I$35</c:f>
+              <c:f>Cumulative!$I$2:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2312,7 +2312,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$K$2:$K$35</c:f>
+              <c:f>Cumulative!$K$2:$K$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2432,7 +2432,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$L$1</c:f>
+              <c:f>Cumulative!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2443,7 +2443,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$I$2:$I$35</c:f>
+              <c:f>Cumulative!$I$2:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2554,7 +2554,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$L$2:$L$35</c:f>
+              <c:f>Cumulative!$L$2:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2674,7 +2674,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$M$1</c:f>
+              <c:f>Cumulative!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2690,7 +2690,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$I$2:$I$35</c:f>
+              <c:f>Cumulative!$I$2:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2801,7 +2801,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$M$2:$M$35</c:f>
+              <c:f>Cumulative!$M$2:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2921,7 +2921,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cumulative 2019-02'!$N$1</c:f>
+              <c:f>Cumulative!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2932,7 +2932,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$I$2:$I$35</c:f>
+              <c:f>Cumulative!$I$2:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="34"/>
@@ -3043,7 +3043,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cumulative 2019-02'!$N$2:$N$35</c:f>
+              <c:f>Cumulative!$N$2:$N$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="34"/>
@@ -6943,9 +6943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>